<commit_message>
Testes corrigidos e atualizados!
</commit_message>
<xml_diff>
--- a/cypress/downloads/relatorio_doacoes.xlsx
+++ b/cypress/downloads/relatorio_doacoes.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,6 +893,358 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sam.abreugouveia@gmail.com</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>(81) 99899-1917</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Plástico</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Gostaria de doar plástico</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>26/11/2024 17:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sam.abreugouveia@gmail.com</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>(81) 99899-1917</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Plástico</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Eu gostaria de doar plástico</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>26/11/2024 17:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>26/11/2024 17:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>26/11/2024 17:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>26/11/2024 17:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>26/11/2024 17:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>26/11/2024 17:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>26/11/2024 17:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>26/11/2024 18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>26/11/2024 18:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Doador</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>doador@gmail.com</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>(81) 99999-9999</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Resíduos têxteis</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Gostaria de fazer uma doação de resíduos têxteis para a confecção de novos brinquedos.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>26/11/2024 18:22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>